<commit_message>
ome minor changes and blacken the letters in Excel-created figures
</commit_message>
<xml_diff>
--- a/TeX/PARCO/Review/MultiThreading.xlsx
+++ b/TeX/PARCO/Review/MultiThreading.xlsx
@@ -8,35 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsushi/AICS/Projects/Survey/Surveys/GIT/MPIsurvey/TeX/PARCO/Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27107A0E-B039-2040-8265-EDA9910431B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14E4282-024E-C04C-9ED4-B73FBA168439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="1060" windowWidth="24140" windowHeight="16480" activeTab="2" xr2:uid="{49B986CD-6A7C-034E-A57E-9643E0D9B6C5}"/>
+    <workbookView xWindow="260" yWindow="1060" windowWidth="24140" windowHeight="16480" activeTab="1" xr2:uid="{49B986CD-6A7C-034E-A57E-9643E0D9B6C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$F$14</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$F$15</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$K$14</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$K$15</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$L$14</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$L$15</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$M$14</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$M$15</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$N$14</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$N$15</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$G$14</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$G$15</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$H$14</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$H$15</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$I$14</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$I$15</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$J$14</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$J$15</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1319,10 +1299,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2233,10 +2210,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2292,10 +2266,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2345,10 +2316,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3279,10 +3247,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3338,10 +3303,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3391,10 +3353,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -5838,7 +5797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219F2E11-C5A3-564B-B4C0-E27BD3D79DF9}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
@@ -5984,8 +5943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF19AAF5-B5B5-A04D-9A65-E5A51A5F45E4}">
   <dimension ref="B3:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="B5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>